<commit_message>
feat: Adicionadas as funções das opções 4 e 5
</commit_message>
<xml_diff>
--- a/salas_reservadas.xlsx
+++ b/salas_reservadas.xlsx
@@ -475,12 +475,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Esdras (Onibus I)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Esdras (Onibus I)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1376,12 +1376,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>lowfrei (cabacisse)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>lowfrei (cabacisse)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>

<commit_message>
refactor: Corrigido erro de exibição dos horarios
</commit_message>
<xml_diff>
--- a/salas_reservadas.xlsx
+++ b/salas_reservadas.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Segunda" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Terça" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Quarta" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Quinta" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sexta" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Segunda" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Terça" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Quarta" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Quinta" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sexta" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,12 +475,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Esdras (Onibus I)</t>
+          <t>Ana Souza (Banco de Dados)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Esdras (Onibus I)</t>
+          <t>Ana Souza (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Algoritmos)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -525,12 +525,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>sovas (resenha)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>sovas (resenha)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
     </row>
@@ -705,12 +705,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Sistemas Operacionais)</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Algoritmos)</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Algoritmos)</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Redes de Computadores)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Redes de Computadores)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Algoritmos)</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1376,12 +1376,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>lowfrei (cabacisse)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>lowfrei (cabacisse)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Banco de Dados)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1416,12 +1416,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Banco de Dados)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Algoritmos)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Algoritmos)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1712,12 +1712,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Algoritmos)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1732,12 +1732,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>asdf (asdf)</t>
+          <t>Juliana Costa (Algoritmos)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>asdf (asdf)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1857,12 +1857,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Estruturas de Dados)</t>
         </is>
       </c>
     </row>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lowfrei (Tomar nota I)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Algoritmos)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2122,12 +2122,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Algoritmos)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Algoritmos)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Redes de Computadores)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Banco de Dados)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Algoritmos)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Algoritmos)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Algoritmos)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Estruturas de Dados)</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Banco de Dados)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Banco de Dados)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Banco de Dados)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Redes de Computadores)</t>
         </is>
       </c>
     </row>
@@ -3074,7 +3074,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Redes de Computadores)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lucas Ribeiro (Redes de Computadores)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -3214,7 +3214,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Carlos Silva (Algoritmos)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Banco de Dados)</t>
         </is>
       </c>
     </row>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Pedro Mendes (Sistemas Operacionais)</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Algoritmos)</t>
         </is>
       </c>
     </row>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Juliana Costa (Estruturas de Dados)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ana Souza (Sistemas Operacionais)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">

</xml_diff>